<commit_message>
WEEK 05-04 last edit
</commit_message>
<xml_diff>
--- a/WEEK formos/WEEK 05-04.xlsx
+++ b/WEEK formos/WEEK 05-04.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaponnik\Desktop\git repos\TSP\WEEK formos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{085AF6F5-90B1-435E-A1FF-D294238AE6EC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week" sheetId="1" r:id="rId1"/>
@@ -34,7 +40,7 @@
     <definedName name="validTeamMembersInitials">[1]Team!$C$2:$C$21</definedName>
     <definedName name="WEEKData">Week!$G$7:$G$11,Week!$I$7:$I$11,Week!$C$15:$C$20,Week!$E$15:$E$20,Week!$G$15:$G$20,Week!$I$15:$I$20</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -166,7 +172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -379,11 +385,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -391,6 +400,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -907,19 +922,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="WeekSummary"/>
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>